<commit_message>
adds GDPR principles (Art.5) to EU-GDPR
- adds gdpr principles from Art.5 as instances of dpv:Principle
- adds property dpv:hasRecordOfActivity to TOMs
</commit_message>
<xml_diff>
--- a/code/vocab_csv/eu-gdpr.xlsx
+++ b/code/vocab_csv/eu-gdpr.xlsx
@@ -12,9 +12,10 @@
     <sheet state="visible" name="GDPR_DPIA" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="GDPR_DPIA_properties" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="GDPR_compliance" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="GDPR_entities" sheetId="10" r:id="rId13"/>
-    <sheet state="visible" name="GDPR_entities_properties" sheetId="11" r:id="rId14"/>
-    <sheet state="visible" name="GDPR_Justifications" sheetId="12" r:id="rId15"/>
+    <sheet state="visible" name="GDPR_principles" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="GDPR_entities" sheetId="11" r:id="rId14"/>
+    <sheet state="visible" name="GDPR_entities_properties" sheetId="12" r:id="rId15"/>
+    <sheet state="visible" name="GDPR_Justifications" sheetId="13" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1634" uniqueCount="688">
   <si>
     <t>Term</t>
   </si>
@@ -1620,6 +1621,114 @@
     <t>The systematic and extensive evaluation of personal aspects</t>
   </si>
   <si>
+    <t>GDPR Principles from Art.5</t>
+  </si>
+  <si>
+    <t>LawfulnessPrinciple</t>
+  </si>
+  <si>
+    <t>Lawfulness Principle</t>
+  </si>
+  <si>
+    <t>Principle stating personal data must be processed processed in a lawfull manner in relation to the data subject</t>
+  </si>
+  <si>
+    <t>dpv:Principle</t>
+  </si>
+  <si>
+    <t>GDPR Art.5-1a</t>
+  </si>
+  <si>
+    <t>TransparencyPrinciple</t>
+  </si>
+  <si>
+    <t>Transparency Principle</t>
+  </si>
+  <si>
+    <t>Principle stating personal data must be processed processed in a transparent manner in relation to the data subject</t>
+  </si>
+  <si>
+    <t>FairnessPrinciple</t>
+  </si>
+  <si>
+    <t>Fairness Principle</t>
+  </si>
+  <si>
+    <t>Principle stating personal data must be processed processed fairly in relation to the data subject</t>
+  </si>
+  <si>
+    <t>PurposeLimitationPrinciple</t>
+  </si>
+  <si>
+    <t>PurposeLimitation Principle</t>
+  </si>
+  <si>
+    <t>Principle stating personal data collected for specified, explicit and legitimate purposes and not further processed in a manner that is incompatible with those purposes; further processing for archiving purposes in the public interest, scientific or historical research purposes or statistical purposes shall, in accordance with Article 89(1), not be considered to be incompatible with the initial purposes</t>
+  </si>
+  <si>
+    <t>GDPR Art.5-1b</t>
+  </si>
+  <si>
+    <t>DataMinimisationPrinciple</t>
+  </si>
+  <si>
+    <t>DataMinimisation Principle</t>
+  </si>
+  <si>
+    <t>Principle stating personal data must be processed adequate, relevant and limited to what is necessary in relation to the purposes for which they are processed</t>
+  </si>
+  <si>
+    <t>GDPR Art.5-1c</t>
+  </si>
+  <si>
+    <t>AccuracyPrinciple</t>
+  </si>
+  <si>
+    <t>Accuracy Principle</t>
+  </si>
+  <si>
+    <t>Principle stating personal data must be accurate and, where necessary, kept up to date; every reasonable step must be taken to ensure that personal data that are inaccurate, having regard to the purposes for which they are processed, are erased or rectified without delay used for</t>
+  </si>
+  <si>
+    <t>GDPR Art.5-1d</t>
+  </si>
+  <si>
+    <t>StorageLimitationPrinciple</t>
+  </si>
+  <si>
+    <t>StorageLimitation Principle</t>
+  </si>
+  <si>
+    <t>Principle stating personal data must be kept in a form which permits identification of data subjects for no longer than is necessary for the purposes for which the personal data are processed; personal data may be stored for longer periods insofar as the personal data will be processed solely for archiving purposes in the public interest, scientific or historical research purposes or statistical purposes in accordance with Article 89(1) subject to implementation of the appropriate technical and organisational measures required by this Regulation in order to safeguard the rights and freedoms of the data subject</t>
+  </si>
+  <si>
+    <t>GDPR Art.5-1e</t>
+  </si>
+  <si>
+    <t>IntegrityConfidentialityPrinciple</t>
+  </si>
+  <si>
+    <t>IntegrityConfidentiality Principle</t>
+  </si>
+  <si>
+    <t>Principle stating personal data must be processed in a manner that ensures appropriate security of the personal data, including protection against unauthorised or unlawful processing and against accidental loss, destruction or damage, using appropriate technical or organisational measures</t>
+  </si>
+  <si>
+    <t>GDPR Art.5-1f</t>
+  </si>
+  <si>
+    <t>AccountabilityPrinciple</t>
+  </si>
+  <si>
+    <t>Accountability Principle</t>
+  </si>
+  <si>
+    <t>Principle stating the controller shall be responsible for, and be able to demonstrate compliance with the other principles (from Art.5-1)</t>
+  </si>
+  <si>
+    <t>GDPR Art.5-2</t>
+  </si>
+  <si>
     <t>Authorities</t>
   </si>
   <si>
@@ -2102,7 +2211,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2229,6 +2338,10 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color rgb="FF0000FF"/>
+      <name val="&quot;Arial&quot;"/>
+    </font>
+    <font>
       <i/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -2316,7 +2429,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="79">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2505,16 +2618,40 @@
     <xf borderId="0" fillId="4" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2590,6 +2727,10 @@
 </file>
 
 <file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -3814,6 +3955,610 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="69" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="70" t="s">
+        <v>498</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="71" t="s">
+        <v>499</v>
+      </c>
+      <c r="B3" s="71" t="s">
+        <v>500</v>
+      </c>
+      <c r="C3" s="71" t="s">
+        <v>501</v>
+      </c>
+      <c r="D3" s="71" t="s">
+        <v>502</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>299</v>
+      </c>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="72" t="s">
+        <v>503</v>
+      </c>
+      <c r="K3" s="73">
+        <v>45424.0</v>
+      </c>
+      <c r="L3" s="54"/>
+      <c r="M3" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="55"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
+      <c r="AB3" s="54"/>
+      <c r="AC3" s="54"/>
+      <c r="AD3" s="54"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="71" t="s">
+        <v>504</v>
+      </c>
+      <c r="B4" s="71" t="s">
+        <v>505</v>
+      </c>
+      <c r="C4" s="71" t="s">
+        <v>506</v>
+      </c>
+      <c r="D4" s="71" t="s">
+        <v>502</v>
+      </c>
+      <c r="E4" s="71" t="s">
+        <v>299</v>
+      </c>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="72" t="s">
+        <v>503</v>
+      </c>
+      <c r="K4" s="73">
+        <v>45424.0</v>
+      </c>
+      <c r="L4" s="54"/>
+      <c r="M4" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="55"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="54"/>
+      <c r="T4" s="54"/>
+      <c r="U4" s="54"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="54"/>
+      <c r="X4" s="54"/>
+      <c r="Y4" s="54"/>
+      <c r="Z4" s="54"/>
+      <c r="AA4" s="54"/>
+      <c r="AB4" s="54"/>
+      <c r="AC4" s="54"/>
+      <c r="AD4" s="54"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="71" t="s">
+        <v>507</v>
+      </c>
+      <c r="B5" s="71" t="s">
+        <v>508</v>
+      </c>
+      <c r="C5" s="74" t="s">
+        <v>509</v>
+      </c>
+      <c r="D5" s="71" t="s">
+        <v>502</v>
+      </c>
+      <c r="E5" s="71" t="s">
+        <v>299</v>
+      </c>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="72" t="s">
+        <v>503</v>
+      </c>
+      <c r="K5" s="73">
+        <v>45424.0</v>
+      </c>
+      <c r="L5" s="54"/>
+      <c r="M5" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" s="55"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="54"/>
+      <c r="S5" s="54"/>
+      <c r="T5" s="54"/>
+      <c r="U5" s="54"/>
+      <c r="V5" s="54"/>
+      <c r="W5" s="54"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="54"/>
+      <c r="AB5" s="54"/>
+      <c r="AC5" s="54"/>
+      <c r="AD5" s="54"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="71" t="s">
+        <v>510</v>
+      </c>
+      <c r="B6" s="71" t="s">
+        <v>511</v>
+      </c>
+      <c r="C6" s="72" t="s">
+        <v>512</v>
+      </c>
+      <c r="D6" s="71" t="s">
+        <v>502</v>
+      </c>
+      <c r="E6" s="71" t="s">
+        <v>299</v>
+      </c>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="72" t="s">
+        <v>513</v>
+      </c>
+      <c r="K6" s="73">
+        <v>45424.0</v>
+      </c>
+      <c r="L6" s="54"/>
+      <c r="M6" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" s="55"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
+      <c r="T6" s="54"/>
+      <c r="U6" s="54"/>
+      <c r="V6" s="54"/>
+      <c r="W6" s="54"/>
+      <c r="X6" s="54"/>
+      <c r="Y6" s="54"/>
+      <c r="Z6" s="54"/>
+      <c r="AA6" s="54"/>
+      <c r="AB6" s="54"/>
+      <c r="AC6" s="54"/>
+      <c r="AD6" s="54"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="s">
+        <v>514</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>515</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>516</v>
+      </c>
+      <c r="D7" s="71" t="s">
+        <v>502</v>
+      </c>
+      <c r="E7" s="71" t="s">
+        <v>299</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="72" t="s">
+        <v>517</v>
+      </c>
+      <c r="K7" s="73">
+        <v>45424.0</v>
+      </c>
+      <c r="L7" s="11"/>
+      <c r="M7" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="O7" s="47"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>519</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>520</v>
+      </c>
+      <c r="D8" s="71" t="s">
+        <v>502</v>
+      </c>
+      <c r="E8" s="71" t="s">
+        <v>299</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="72" t="s">
+        <v>521</v>
+      </c>
+      <c r="K8" s="73">
+        <v>45424.0</v>
+      </c>
+      <c r="L8" s="11"/>
+      <c r="M8" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="O8" s="47"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="11"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="s">
+        <v>522</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>523</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>524</v>
+      </c>
+      <c r="D9" s="71" t="s">
+        <v>502</v>
+      </c>
+      <c r="E9" s="71" t="s">
+        <v>299</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="72" t="s">
+        <v>525</v>
+      </c>
+      <c r="K9" s="73">
+        <v>45424.0</v>
+      </c>
+      <c r="L9" s="11"/>
+      <c r="M9" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="O9" s="47"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="11"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="s">
+        <v>526</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>527</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>528</v>
+      </c>
+      <c r="D10" s="71" t="s">
+        <v>502</v>
+      </c>
+      <c r="E10" s="71" t="s">
+        <v>299</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="72" t="s">
+        <v>529</v>
+      </c>
+      <c r="K10" s="73">
+        <v>45424.0</v>
+      </c>
+      <c r="L10" s="11"/>
+      <c r="M10" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10" s="47"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="s">
+        <v>530</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>531</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>532</v>
+      </c>
+      <c r="D11" s="71" t="s">
+        <v>502</v>
+      </c>
+      <c r="E11" s="71" t="s">
+        <v>299</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="72" t="s">
+        <v>533</v>
+      </c>
+      <c r="K11" s="73">
+        <v>45424.0</v>
+      </c>
+      <c r="L11" s="11"/>
+      <c r="M11" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="O11" s="47"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+    </row>
+    <row r="12">
+      <c r="J12" s="72"/>
+      <c r="K12" s="13"/>
+      <c r="O12" s="47"/>
+    </row>
+    <row r="13">
+      <c r="K13" s="13"/>
+      <c r="O13" s="47"/>
+    </row>
+    <row r="14">
+      <c r="K14" s="13"/>
+      <c r="O14" s="47"/>
+    </row>
+    <row r="15">
+      <c r="K15" s="13"/>
+      <c r="O15" s="47"/>
+    </row>
+    <row r="16">
+      <c r="K16" s="13"/>
+    </row>
+    <row r="17">
+      <c r="K17" s="13"/>
+    </row>
+    <row r="18">
+      <c r="K18" s="13"/>
+    </row>
+    <row r="19">
+      <c r="K19" s="13"/>
+    </row>
+    <row r="20">
+      <c r="K20" s="13"/>
+    </row>
+    <row r="21">
+      <c r="K21" s="13"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:AD50">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$M2="accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:AD50">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$M2="proposed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:AD50">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$M2="changed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="32.13"/>
+    <col customWidth="1" min="2" max="2" width="20.88"/>
+    <col customWidth="1" min="3" max="3" width="38.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="28.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3862,7 +4607,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>498</v>
+        <v>534</v>
       </c>
       <c r="C2" s="38"/>
       <c r="J2" s="47"/>
@@ -3871,16 +4616,16 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>499</v>
+        <v>535</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>500</v>
+        <v>536</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>501</v>
+        <v>537</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>502</v>
+        <v>538</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>383</v>
@@ -3890,7 +4635,7 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="10" t="s">
-        <v>503</v>
+        <v>539</v>
       </c>
       <c r="K3" s="13"/>
       <c r="L3" s="11"/>
@@ -3919,16 +4664,16 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>504</v>
+        <v>540</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>505</v>
+        <v>541</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>506</v>
+        <v>542</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>502</v>
+        <v>538</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>383</v>
@@ -3938,7 +4683,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="10" t="s">
-        <v>503</v>
+        <v>539</v>
       </c>
       <c r="K4" s="13"/>
       <c r="L4" s="11"/>
@@ -3967,16 +4712,16 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>507</v>
+        <v>543</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>508</v>
+        <v>544</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>509</v>
+        <v>545</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>502</v>
+        <v>538</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>383</v>
@@ -3986,7 +4731,7 @@
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="10" t="s">
-        <v>503</v>
+        <v>539</v>
       </c>
       <c r="K5" s="13"/>
       <c r="L5" s="11"/>
@@ -4020,23 +4765,23 @@
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>510</v>
+        <v>546</v>
       </c>
       <c r="K7" s="13"/>
       <c r="O7" s="47"/>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>511</v>
+        <v>547</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>511</v>
+        <v>547</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>512</v>
+        <v>548</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>513</v>
+        <v>549</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>383</v>
@@ -4046,7 +4791,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="10" t="s">
-        <v>514</v>
+        <v>550</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="11"/>
@@ -4075,16 +4820,16 @@
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>515</v>
+        <v>551</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>516</v>
+        <v>552</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>517</v>
+        <v>553</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>518</v>
+        <v>554</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>383</v>
@@ -4094,7 +4839,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="10" t="s">
-        <v>519</v>
+        <v>555</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="11"/>
@@ -4123,16 +4868,16 @@
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>520</v>
+        <v>556</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>521</v>
+        <v>557</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>522</v>
+        <v>558</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>518</v>
+        <v>554</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>383</v>
@@ -4142,7 +4887,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="10" t="s">
-        <v>523</v>
+        <v>559</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="11"/>
@@ -4201,7 +4946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4273,28 +5018,28 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>524</v>
+        <v>560</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>525</v>
+        <v>561</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>526</v>
+        <v>562</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>527</v>
+        <v>563</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>527</v>
+        <v>563</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>528</v>
+        <v>564</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="10" t="s">
-        <v>503</v>
+        <v>539</v>
       </c>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
@@ -4321,28 +5066,28 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>529</v>
+        <v>565</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>530</v>
+        <v>566</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>531</v>
+        <v>567</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>527</v>
+        <v>563</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>527</v>
+        <v>563</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>528</v>
+        <v>564</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="10" t="s">
-        <v>503</v>
+        <v>539</v>
       </c>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
@@ -4369,28 +5114,28 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>532</v>
+        <v>568</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>533</v>
+        <v>569</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>534</v>
+        <v>570</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>527</v>
+        <v>563</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>527</v>
+        <v>563</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>528</v>
+        <v>564</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="10" t="s">
-        <v>503</v>
+        <v>539</v>
       </c>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
@@ -4417,28 +5162,28 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>535</v>
+        <v>571</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>536</v>
+        <v>572</v>
       </c>
       <c r="C5" s="51" t="s">
-        <v>537</v>
+        <v>573</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>574</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>538</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>502</v>
-      </c>
       <c r="F5" s="10" t="s">
-        <v>528</v>
+        <v>564</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="10" t="s">
-        <v>503</v>
+        <v>539</v>
       </c>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
@@ -4465,28 +5210,28 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>539</v>
+        <v>575</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>540</v>
+        <v>576</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>541</v>
+        <v>577</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>574</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>538</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>502</v>
-      </c>
       <c r="F6" s="10" t="s">
-        <v>528</v>
+        <v>564</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="10" t="s">
-        <v>503</v>
+        <v>539</v>
       </c>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
@@ -4513,28 +5258,28 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>542</v>
+        <v>578</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>543</v>
+        <v>579</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>544</v>
+        <v>580</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>574</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>538</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>502</v>
-      </c>
       <c r="F7" s="10" t="s">
-        <v>528</v>
+        <v>564</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="10" t="s">
-        <v>503</v>
+        <v>539</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
@@ -7572,7 +8317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -7609,7 +8354,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>545</v>
+        <v>581</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -7641,10 +8386,10 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>546</v>
-      </c>
-      <c r="B2" s="66" t="s">
-        <v>547</v>
+        <v>582</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>583</v>
       </c>
       <c r="C2" s="38"/>
       <c r="J2" s="47"/>
@@ -7653,61 +8398,61 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>549</v>
+        <v>585</v>
       </c>
       <c r="K3" s="13"/>
       <c r="O3" s="47"/>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>550</v>
+        <v>586</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>551</v>
+        <v>587</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>552</v>
+        <v>588</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="K4" s="13"/>
       <c r="O4" s="47"/>
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>553</v>
+        <v>589</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>554</v>
+        <v>590</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>555</v>
+        <v>591</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="K5" s="13"/>
       <c r="O5" s="47"/>
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>556</v>
+        <v>592</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>557</v>
+        <v>593</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>558</v>
+        <v>594</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="K6" s="13"/>
       <c r="O6" s="47"/>
@@ -7721,10 +8466,10 @@
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
-        <v>559</v>
-      </c>
-      <c r="B8" s="66" t="s">
-        <v>560</v>
+        <v>595</v>
+      </c>
+      <c r="B8" s="75" t="s">
+        <v>596</v>
       </c>
       <c r="C8" s="10"/>
       <c r="K8" s="13"/>
@@ -7732,57 +8477,57 @@
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>561</v>
+        <v>597</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>562</v>
+        <v>598</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>563</v>
+        <v>599</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>550</v>
+        <v>586</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="K9" s="13"/>
       <c r="O9" s="47"/>
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>564</v>
+        <v>600</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>565</v>
+        <v>601</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>566</v>
+        <v>602</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>553</v>
+        <v>589</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="K10" s="13"/>
       <c r="O10" s="47"/>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>567</v>
+        <v>603</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>568</v>
+        <v>604</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>569</v>
+        <v>605</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>556</v>
+        <v>592</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="K11" s="13"/>
       <c r="O11" s="47"/>
@@ -7796,10 +8541,10 @@
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>570</v>
-      </c>
-      <c r="B13" s="66" t="s">
-        <v>571</v>
+        <v>606</v>
+      </c>
+      <c r="B13" s="75" t="s">
+        <v>607</v>
       </c>
       <c r="C13" s="10"/>
       <c r="J13" s="10"/>
@@ -7807,152 +8552,152 @@
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>572</v>
+        <v>608</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>573</v>
+        <v>609</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>574</v>
+        <v>610</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>550</v>
+        <v>586</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>575</v>
+        <v>611</v>
       </c>
       <c r="K14" s="13"/>
     </row>
     <row r="15">
       <c r="A15" s="10" t="s">
-        <v>576</v>
+        <v>612</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>577</v>
+        <v>613</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>578</v>
+        <v>614</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>550</v>
+        <v>586</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>579</v>
+        <v>615</v>
       </c>
       <c r="K15" s="13"/>
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
-        <v>580</v>
+        <v>616</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>581</v>
+        <v>617</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>582</v>
+        <v>618</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>550</v>
+        <v>586</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>579</v>
+        <v>615</v>
       </c>
       <c r="K16" s="13"/>
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
-        <v>583</v>
+        <v>619</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>621</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>586</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>584</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>585</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>550</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>548</v>
-      </c>
       <c r="J17" s="10" t="s">
-        <v>579</v>
+        <v>615</v>
       </c>
       <c r="K17" s="13"/>
     </row>
     <row r="18">
       <c r="A18" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>623</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>624</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>586</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>587</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>550</v>
-      </c>
       <c r="E18" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>589</v>
+        <v>625</v>
       </c>
       <c r="K18" s="13"/>
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>590</v>
+        <v>626</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>591</v>
+        <v>627</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>592</v>
+        <v>628</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>550</v>
+        <v>586</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>593</v>
+        <v>629</v>
       </c>
       <c r="K19" s="13"/>
     </row>
     <row r="20">
-      <c r="A20" s="67" t="s">
-        <v>594</v>
-      </c>
-      <c r="B20" s="67" t="s">
-        <v>595</v>
-      </c>
-      <c r="C20" s="68" t="s">
-        <v>596</v>
+      <c r="A20" s="72" t="s">
+        <v>630</v>
+      </c>
+      <c r="B20" s="72" t="s">
+        <v>631</v>
+      </c>
+      <c r="C20" s="76" t="s">
+        <v>632</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>550</v>
+        <v>586</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="F20" s="54"/>
       <c r="G20" s="54"/>
       <c r="H20" s="54"/>
       <c r="I20" s="54"/>
-      <c r="J20" s="69" t="s">
-        <v>597</v>
+      <c r="J20" s="77" t="s">
+        <v>633</v>
       </c>
       <c r="K20" s="54"/>
       <c r="L20" s="54"/>
@@ -7976,27 +8721,27 @@
       <c r="AD20" s="54"/>
     </row>
     <row r="21">
-      <c r="A21" s="67" t="s">
-        <v>598</v>
-      </c>
-      <c r="B21" s="67" t="s">
-        <v>599</v>
-      </c>
-      <c r="C21" s="70" t="s">
-        <v>600</v>
+      <c r="A21" s="72" t="s">
+        <v>634</v>
+      </c>
+      <c r="B21" s="72" t="s">
+        <v>635</v>
+      </c>
+      <c r="C21" s="78" t="s">
+        <v>636</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>550</v>
+        <v>586</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="F21" s="54"/>
       <c r="G21" s="54"/>
       <c r="H21" s="54"/>
       <c r="I21" s="54"/>
-      <c r="J21" s="68" t="s">
-        <v>601</v>
+      <c r="J21" s="76" t="s">
+        <v>637</v>
       </c>
       <c r="K21" s="54"/>
       <c r="L21" s="54"/>
@@ -8020,27 +8765,27 @@
       <c r="AD21" s="54"/>
     </row>
     <row r="22">
-      <c r="A22" s="67" t="s">
-        <v>602</v>
-      </c>
-      <c r="B22" s="67" t="s">
-        <v>603</v>
+      <c r="A22" s="72" t="s">
+        <v>638</v>
+      </c>
+      <c r="B22" s="72" t="s">
+        <v>639</v>
       </c>
       <c r="C22" s="54" t="s">
-        <v>604</v>
+        <v>640</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>550</v>
+        <v>586</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="F22" s="54"/>
       <c r="G22" s="54"/>
       <c r="H22" s="54"/>
       <c r="I22" s="54"/>
-      <c r="J22" s="68" t="s">
-        <v>605</v>
+      <c r="J22" s="76" t="s">
+        <v>641</v>
       </c>
       <c r="K22" s="54"/>
       <c r="L22" s="54"/>
@@ -8065,243 +8810,243 @@
     </row>
     <row r="23">
       <c r="A23" s="10" t="s">
-        <v>606</v>
+        <v>642</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>607</v>
+        <v>643</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>608</v>
+        <v>644</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>550</v>
+        <v>586</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>548</v>
-      </c>
-      <c r="J23" s="68" t="s">
-        <v>609</v>
+        <v>584</v>
+      </c>
+      <c r="J23" s="76" t="s">
+        <v>645</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="s">
-        <v>610</v>
+        <v>646</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>611</v>
+        <v>647</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>612</v>
+        <v>648</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>550</v>
+        <v>586</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>613</v>
+        <v>649</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8"/>
-      <c r="B25" s="66"/>
+      <c r="B25" s="75"/>
       <c r="C25" s="10"/>
       <c r="J25" s="10"/>
     </row>
     <row r="26">
       <c r="A26" s="8" t="s">
-        <v>614</v>
-      </c>
-      <c r="B26" s="66" t="s">
-        <v>571</v>
+        <v>650</v>
+      </c>
+      <c r="B26" s="75" t="s">
+        <v>607</v>
       </c>
       <c r="C26" s="10"/>
       <c r="J26" s="10"/>
     </row>
     <row r="27">
       <c r="A27" s="10" t="s">
-        <v>615</v>
+        <v>651</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>616</v>
+        <v>652</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>617</v>
+        <v>653</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>556</v>
+        <v>592</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>618</v>
+        <v>654</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="10" t="s">
-        <v>619</v>
+        <v>655</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>620</v>
+        <v>656</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>621</v>
+        <v>657</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>556</v>
+        <v>592</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>622</v>
+        <v>658</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="10" t="s">
-        <v>623</v>
+        <v>659</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>624</v>
+        <v>660</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>625</v>
+        <v>661</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>556</v>
+        <v>592</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>622</v>
+        <v>658</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="10" t="s">
-        <v>626</v>
+        <v>662</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>627</v>
+        <v>663</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>628</v>
+        <v>664</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>556</v>
+        <v>592</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J30" s="48" t="s">
-        <v>629</v>
+        <v>665</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="8" t="s">
-        <v>630</v>
+        <v>666</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="10" t="s">
-        <v>631</v>
+        <v>667</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>632</v>
+        <v>668</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>633</v>
+        <v>669</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>634</v>
+        <v>670</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>635</v>
+        <v>671</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="10" t="s">
-        <v>636</v>
+        <v>672</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>637</v>
+        <v>673</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>638</v>
+        <v>674</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>634</v>
+        <v>670</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>639</v>
+        <v>675</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="10" t="s">
-        <v>640</v>
+        <v>676</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>641</v>
+        <v>677</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>642</v>
+        <v>678</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>634</v>
+        <v>670</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>643</v>
+        <v>679</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="10" t="s">
-        <v>644</v>
+        <v>680</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>645</v>
+        <v>681</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>646</v>
+        <v>682</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>634</v>
+        <v>670</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>647</v>
+        <v>683</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="10" t="s">
-        <v>648</v>
+        <v>684</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>649</v>
+        <v>685</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>650</v>
+        <v>686</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>634</v>
+        <v>670</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>651</v>
+        <v>687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds EU GDPR documentation; fixes breach concepts
- adds documentation for EU GDPR (diagrams missing), some examples
  added, and notes added mentioning upcoming guidance for DPIA and Data
  Breach incicent management
- fixes issue where data breach notices for DPA were not grouped in a
  hierarchy due to missing parent
</commit_message>
<xml_diff>
--- a/code/vocab_csv/eu-gdpr.xlsx
+++ b/code/vocab_csv/eu-gdpr.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1850" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1853" uniqueCount="793">
   <si>
     <t>Term</t>
   </si>
@@ -1752,6 +1752,9 @@
   </si>
   <si>
     <t>Notice sent by a Controller within 72 hours of becoming aware of a personal data breach to the competent DPA, with justifications provided where the notice is made after 72 hours</t>
+  </si>
+  <si>
+    <t>eu-gdpr:DPABreachNotice</t>
   </si>
   <si>
     <t>DPAPhasedBreachNotice</t>
@@ -4347,7 +4350,7 @@
     </row>
     <row r="2">
       <c r="A2" s="62" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B2" s="63"/>
       <c r="C2" s="63"/>
@@ -4381,17 +4384,17 @@
     </row>
     <row r="3">
       <c r="A3" s="66" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B3" s="67" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C3" s="68" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="D3" s="69"/>
       <c r="E3" s="68" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="F3" s="70"/>
       <c r="G3" s="70"/>
@@ -4427,19 +4430,19 @@
     </row>
     <row r="4">
       <c r="A4" s="69" t="s">
+        <v>587</v>
+      </c>
+      <c r="B4" s="74" t="s">
+        <v>588</v>
+      </c>
+      <c r="C4" s="69" t="s">
+        <v>589</v>
+      </c>
+      <c r="D4" s="68" t="s">
+        <v>590</v>
+      </c>
+      <c r="E4" s="68" t="s">
         <v>586</v>
-      </c>
-      <c r="B4" s="74" t="s">
-        <v>587</v>
-      </c>
-      <c r="C4" s="69" t="s">
-        <v>588</v>
-      </c>
-      <c r="D4" s="68" t="s">
-        <v>589</v>
-      </c>
-      <c r="E4" s="68" t="s">
-        <v>585</v>
       </c>
       <c r="F4" s="70"/>
       <c r="G4" s="70"/>
@@ -4475,19 +4478,19 @@
     </row>
     <row r="5">
       <c r="A5" s="69" t="s">
+        <v>591</v>
+      </c>
+      <c r="B5" s="74" t="s">
+        <v>592</v>
+      </c>
+      <c r="C5" s="69" t="s">
+        <v>593</v>
+      </c>
+      <c r="D5" s="68" t="s">
         <v>590</v>
       </c>
-      <c r="B5" s="74" t="s">
-        <v>591</v>
-      </c>
-      <c r="C5" s="69" t="s">
-        <v>592</v>
-      </c>
-      <c r="D5" s="68" t="s">
-        <v>589</v>
-      </c>
       <c r="E5" s="68" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="F5" s="70"/>
       <c r="G5" s="70"/>
@@ -4523,19 +4526,19 @@
     </row>
     <row r="6">
       <c r="A6" s="68" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B6" s="73" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C6" s="73" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="D6" s="68" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="E6" s="68" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="F6" s="70"/>
       <c r="G6" s="70"/>
@@ -4576,13 +4579,13 @@
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
@@ -4618,13 +4621,13 @@
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -4790,7 +4793,7 @@
     </row>
     <row r="2">
       <c r="A2" s="79" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B2" s="63"/>
       <c r="C2" s="63"/>
@@ -4824,16 +4827,16 @@
     </row>
     <row r="3">
       <c r="A3" s="80" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B3" s="80" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="C3" s="80" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D3" s="80" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E3" s="80" t="s">
         <v>299</v>
@@ -4843,7 +4846,7 @@
       <c r="H3" s="63"/>
       <c r="I3" s="63"/>
       <c r="J3" s="81" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="K3" s="82">
         <v>45424.0</v>
@@ -4874,16 +4877,16 @@
     </row>
     <row r="4">
       <c r="A4" s="80" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B4" s="80" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C4" s="80" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D4" s="80" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E4" s="80" t="s">
         <v>299</v>
@@ -4893,7 +4896,7 @@
       <c r="H4" s="63"/>
       <c r="I4" s="63"/>
       <c r="J4" s="81" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="K4" s="82">
         <v>45424.0</v>
@@ -4924,16 +4927,16 @@
     </row>
     <row r="5">
       <c r="A5" s="80" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B5" s="80" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C5" s="83" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D5" s="80" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E5" s="80" t="s">
         <v>299</v>
@@ -4943,7 +4946,7 @@
       <c r="H5" s="63"/>
       <c r="I5" s="63"/>
       <c r="J5" s="81" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="K5" s="82">
         <v>45424.0</v>
@@ -4974,16 +4977,16 @@
     </row>
     <row r="6">
       <c r="A6" s="80" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B6" s="80" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C6" s="81" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D6" s="80" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E6" s="80" t="s">
         <v>299</v>
@@ -4993,7 +4996,7 @@
       <c r="H6" s="63"/>
       <c r="I6" s="63"/>
       <c r="J6" s="81" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="K6" s="82">
         <v>45424.0</v>
@@ -5024,16 +5027,16 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D7" s="80" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E7" s="80" t="s">
         <v>299</v>
@@ -5043,7 +5046,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="81" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="K7" s="82">
         <v>45424.0</v>
@@ -5074,16 +5077,16 @@
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D8" s="80" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E8" s="80" t="s">
         <v>299</v>
@@ -5093,7 +5096,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="81" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="K8" s="82">
         <v>45424.0</v>
@@ -5124,16 +5127,16 @@
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="D9" s="80" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E9" s="80" t="s">
         <v>299</v>
@@ -5143,7 +5146,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="81" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="K9" s="82">
         <v>45424.0</v>
@@ -5174,16 +5177,16 @@
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D10" s="80" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E10" s="80" t="s">
         <v>299</v>
@@ -5193,7 +5196,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="81" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="K10" s="82">
         <v>45424.0</v>
@@ -5224,16 +5227,16 @@
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="D11" s="80" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E11" s="80" t="s">
         <v>299</v>
@@ -5243,7 +5246,7 @@
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="81" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="K11" s="82">
         <v>45424.0</v>
@@ -5394,7 +5397,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C2" s="38"/>
       <c r="J2" s="47"/>
@@ -5403,16 +5406,16 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>383</v>
@@ -5422,7 +5425,7 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="10" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K3" s="13"/>
       <c r="L3" s="11"/>
@@ -5451,16 +5454,16 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>383</v>
@@ -5470,7 +5473,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="10" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K4" s="13"/>
       <c r="L4" s="11"/>
@@ -5499,16 +5502,16 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>383</v>
@@ -5518,7 +5521,7 @@
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="10" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K5" s="13"/>
       <c r="L5" s="11"/>
@@ -5552,23 +5555,23 @@
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="K7" s="13"/>
       <c r="O7" s="47"/>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>383</v>
@@ -5578,7 +5581,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="10" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="11"/>
@@ -5607,16 +5610,16 @@
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>383</v>
@@ -5626,7 +5629,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="10" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="11"/>
@@ -5655,16 +5658,16 @@
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>383</v>
@@ -5674,7 +5677,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="10" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="11"/>
@@ -5805,28 +5808,28 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="10" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
@@ -5853,28 +5856,28 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
+        <v>670</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>671</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>672</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>669</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>670</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>671</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>667</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>667</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>668</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="10" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
@@ -5901,28 +5904,28 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="10" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
@@ -5949,28 +5952,28 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="C5" s="51" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="10" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
@@ -5997,28 +6000,28 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>682</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>679</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>680</v>
-      </c>
-      <c r="C6" s="51" t="s">
-        <v>681</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>678</v>
-      </c>
       <c r="E6" s="10" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="10" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
@@ -6045,28 +6048,28 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="10" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
@@ -9141,7 +9144,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -9173,10 +9176,10 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B2" s="84" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="C2" s="38"/>
       <c r="J2" s="47"/>
@@ -9185,61 +9188,61 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="K3" s="13"/>
       <c r="O3" s="47"/>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="K4" s="13"/>
       <c r="O4" s="47"/>
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="K5" s="13"/>
       <c r="O5" s="47"/>
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="K6" s="13"/>
       <c r="O6" s="47"/>
@@ -9253,10 +9256,10 @@
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B8" s="84" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="C8" s="10"/>
       <c r="K8" s="13"/>
@@ -9264,57 +9267,57 @@
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="K9" s="13"/>
       <c r="O9" s="47"/>
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="K10" s="13"/>
       <c r="O10" s="47"/>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="K11" s="13"/>
       <c r="O11" s="47"/>
@@ -9328,10 +9331,10 @@
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B13" s="84" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C13" s="10"/>
       <c r="J13" s="10"/>
@@ -9339,152 +9342,152 @@
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="K14" s="13"/>
     </row>
     <row r="15">
       <c r="A15" s="10" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="K15" s="13"/>
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
+        <v>721</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>722</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>723</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>689</v>
+      </c>
+      <c r="J16" s="10" t="s">
         <v>720</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>721</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>722</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>690</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>688</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>719</v>
       </c>
       <c r="K16" s="13"/>
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="K17" s="13"/>
     </row>
     <row r="18">
       <c r="A18" s="10" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="K18" s="13"/>
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="K19" s="13"/>
     </row>
     <row r="20">
       <c r="A20" s="81" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B20" s="81" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="C20" s="85" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="F20" s="63"/>
       <c r="G20" s="63"/>
       <c r="H20" s="63"/>
       <c r="I20" s="63"/>
       <c r="J20" s="86" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="K20" s="63"/>
       <c r="L20" s="63"/>
@@ -9509,26 +9512,26 @@
     </row>
     <row r="21">
       <c r="A21" s="81" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B21" s="81" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="C21" s="87" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="F21" s="63"/>
       <c r="G21" s="63"/>
       <c r="H21" s="63"/>
       <c r="I21" s="63"/>
       <c r="J21" s="85" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="K21" s="63"/>
       <c r="L21" s="63"/>
@@ -9553,26 +9556,26 @@
     </row>
     <row r="22">
       <c r="A22" s="81" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="B22" s="81" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="F22" s="63"/>
       <c r="G22" s="63"/>
       <c r="H22" s="63"/>
       <c r="I22" s="63"/>
       <c r="J22" s="85" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="K22" s="63"/>
       <c r="L22" s="63"/>
@@ -9597,42 +9600,42 @@
     </row>
     <row r="23">
       <c r="A23" s="10" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J23" s="85" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
     </row>
     <row r="25">
@@ -9643,197 +9646,197 @@
     </row>
     <row r="26">
       <c r="A26" s="8" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B26" s="84" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C26" s="10"/>
       <c r="J26" s="10"/>
     </row>
     <row r="27">
       <c r="A27" s="10" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="10" t="s">
+        <v>764</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>765</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>766</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>697</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>689</v>
+      </c>
+      <c r="J29" s="10" t="s">
         <v>763</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>764</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>765</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>696</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>688</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="10" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J30" s="48" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="8" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="10" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="10" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="10" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="10" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="10" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
   </sheetData>
@@ -22665,7 +22668,9 @@
       <c r="C22" s="38" t="s">
         <v>541</v>
       </c>
-      <c r="D22" s="11"/>
+      <c r="D22" s="10" t="s">
+        <v>542</v>
+      </c>
       <c r="E22" s="10" t="s">
         <v>538</v>
       </c>
@@ -22703,15 +22708,17 @@
     </row>
     <row r="23">
       <c r="A23" s="10" t="s">
+        <v>543</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>544</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>545</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>542</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>543</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>544</v>
-      </c>
-      <c r="D23" s="11"/>
       <c r="E23" s="10" t="s">
         <v>538</v>
       </c>
@@ -22749,15 +22756,17 @@
     </row>
     <row r="24">
       <c r="A24" s="10" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>547</v>
-      </c>
-      <c r="D24" s="11"/>
+        <v>548</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>542</v>
+      </c>
       <c r="E24" s="10" t="s">
         <v>538</v>
       </c>
@@ -22795,13 +22804,13 @@
     </row>
     <row r="25">
       <c r="A25" s="10" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="10" t="s">
@@ -22841,13 +22850,13 @@
     </row>
     <row r="26">
       <c r="A26" s="10" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="10" t="s">
@@ -22887,13 +22896,13 @@
     </row>
     <row r="27">
       <c r="A27" s="10" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="10" t="s">
@@ -22933,16 +22942,16 @@
     </row>
     <row r="29">
       <c r="A29" s="59" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B29" s="60" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C29" s="56" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D29" s="56" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E29" s="56" t="s">
         <v>383</v>
@@ -22981,16 +22990,16 @@
     </row>
     <row r="30">
       <c r="A30" s="56" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B30" s="56" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C30" s="56" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D30" s="61" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E30" s="56" t="s">
         <v>383</v>
@@ -23029,16 +23038,16 @@
     </row>
     <row r="31">
       <c r="A31" s="56" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B31" s="56" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C31" s="56" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D31" s="55" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="E31" s="56" t="s">
         <v>383</v>
@@ -23077,16 +23086,16 @@
     </row>
     <row r="32">
       <c r="A32" s="56" t="s">
+        <v>570</v>
+      </c>
+      <c r="B32" s="56" t="s">
+        <v>571</v>
+      </c>
+      <c r="C32" s="56" t="s">
+        <v>572</v>
+      </c>
+      <c r="D32" s="55" t="s">
         <v>569</v>
-      </c>
-      <c r="B32" s="56" t="s">
-        <v>570</v>
-      </c>
-      <c r="C32" s="56" t="s">
-        <v>571</v>
-      </c>
-      <c r="D32" s="55" t="s">
-        <v>568</v>
       </c>
       <c r="E32" s="56" t="s">
         <v>383</v>
@@ -23125,16 +23134,16 @@
     </row>
     <row r="33">
       <c r="A33" s="56" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B33" s="56" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C33" s="56" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="D33" s="55" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="E33" s="56" t="s">
         <v>383</v>
@@ -23173,16 +23182,16 @@
     </row>
     <row r="35">
       <c r="A35" s="10" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>383</v>
@@ -23192,7 +23201,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
       <c r="J35" s="10" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="K35" s="13">
         <v>45431.0</v>

</xml_diff>

<commit_message>
FIX: DPV Legal Basis Contract concepts/properties
- `ProviderStandardFormContract` and `ConsumerStandardFormContract`
  added broader `StandardFormContract`
- `ContractControl` types changed declaration in spreadsheet to match
  'class' taxonomy type which automatically generates the subject/object
  annotations in the term definition table in HTML
- `hasContractFulfilmentStatus` and `hasContractClauseFulfilmentStatus`
  merged together into `hasContractualFulfilmentStatus` to enable common
  property and a shorter sensible name for contractual clauses. Domain
  and Range are combined as well (union).
- `ContractualClauseFulfilmentState` parent revised so that it correctly
  shows up in the taxonomy of `dpv:ContractStatus` and `dpv:Context` and
  can be used with the corresponding relations
- Includes RDF and HTML outputs
- minor: Updated reference for EU-GDPR data transfer concept to avoid
  random ordering in RDF for multiple references
</commit_message>
<xml_diff>
--- a/code/vocab_csv/eu-gdpr.xlsx
+++ b/code/vocab_csv/eu-gdpr.xlsx
@@ -2243,21 +2243,7 @@
         <color rgb="FF000000"/>
         <u/>
       </rPr>
-      <t>(GDPR Art.46,</t>
-    </r>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>https://eur-lex.europa.eu/eli/reg/2016/679/art_46/pnt_c/oj)</t>
-    </r>
-    <r>
-      <rPr>
-        <color rgb="FF000000"/>
-        <u/>
-      </rPr>
-      <t>,(EDPB Recommendations 01/2020 on Supplementary Measures and Transfer Tools,</t>
+      <t>(GDPR Art.46 and EDPB Recommendations 01/2020 on Supplementary Measures and Transfer Tools,</t>
     </r>
     <r>
       <rPr>
@@ -26789,14 +26775,8 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N4:P4"/>
     <mergeCell ref="N5:P5"/>
     <mergeCell ref="N6:P6"/>
     <mergeCell ref="N7:P7"/>
@@ -26805,13 +26785,19 @@
     <mergeCell ref="N10:P10"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="N12:P12"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N16:P16"/>
     <mergeCell ref="N17:P17"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N18:P18"/>
     <mergeCell ref="N28:P28"/>
     <mergeCell ref="N29:P29"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="N27:P27"/>
   </mergeCells>
   <conditionalFormatting sqref="A39:C40 D39:E49 F39:I40 J39:J49 K39:AF40 F42 F44 F46 F48">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>

<commit_message>
fixes incorrect parents, new SHACL tests
- `290` adds new test to detect incorrect parent via `rdf:type`
- identifies concept violating above test (also in OOPS! as P34)
- AI: previous HTML for 60d1883367f84a75c5842900f04c04ff941aacef
- DEX: Added metadata for `dex:Example` via RDF hook (passes test)
- breaking changes in EU-GDPR and EU-AIAct
- EU-GDPR: fixed parent `risk:RiskConcept` -> `dpv:RiskConcept`
- EU-AIAct: fixed parent `dpv:Capability` -> `tech:Capability`
</commit_message>
<xml_diff>
--- a/code/vocab_csv/eu-gdpr.xlsx
+++ b/code/vocab_csv/eu-gdpr.xlsx
@@ -2001,7 +2001,7 @@
     <t>risk:RightsImpact</t>
   </si>
   <si>
-    <t>risk:RiskConcept</t>
+    <t>dpv:RiskConcept</t>
   </si>
   <si>
     <t>R,C,I</t>
@@ -27231,9 +27231,11 @@
       <c r="L2" s="33">
         <v>45627.0</v>
       </c>
-      <c r="M2" s="33"/>
+      <c r="M2" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N2" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O2" s="29"/>
       <c r="P2" s="29"/>
@@ -27284,9 +27286,11 @@
       <c r="L3" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M3" s="33"/>
+      <c r="M3" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N3" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O3" s="29"/>
       <c r="P3" s="29"/>
@@ -27337,9 +27341,11 @@
       <c r="L4" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M4" s="33"/>
+      <c r="M4" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N4" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O4" s="29"/>
       <c r="P4" s="29"/>
@@ -27390,9 +27396,11 @@
       <c r="L5" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M5" s="33"/>
+      <c r="M5" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N5" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O5" s="29"/>
       <c r="P5" s="29"/>
@@ -27443,9 +27451,11 @@
       <c r="L6" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M6" s="33"/>
+      <c r="M6" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N6" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O6" s="29"/>
       <c r="P6" s="29"/>
@@ -27496,9 +27506,11 @@
       <c r="L7" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M7" s="33"/>
+      <c r="M7" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N7" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O7" s="29"/>
       <c r="P7" s="29"/>
@@ -27549,9 +27561,11 @@
       <c r="L8" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M8" s="33"/>
+      <c r="M8" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N8" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O8" s="29"/>
       <c r="P8" s="29"/>
@@ -27602,9 +27616,11 @@
       <c r="L9" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M9" s="33"/>
+      <c r="M9" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N9" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O9" s="29"/>
       <c r="P9" s="29"/>
@@ -27655,9 +27671,11 @@
       <c r="L10" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M10" s="33"/>
+      <c r="M10" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N10" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O10" s="29"/>
       <c r="P10" s="29"/>
@@ -27708,9 +27726,11 @@
       <c r="L11" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M11" s="33"/>
+      <c r="M11" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N11" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O11" s="29"/>
       <c r="P11" s="29"/>
@@ -27761,9 +27781,11 @@
       <c r="L12" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M12" s="33"/>
+      <c r="M12" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N12" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O12" s="29"/>
       <c r="P12" s="29"/>
@@ -27814,9 +27836,11 @@
       <c r="L13" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M13" s="33"/>
+      <c r="M13" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N13" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O13" s="29"/>
       <c r="P13" s="29"/>
@@ -27867,9 +27891,11 @@
       <c r="L14" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M14" s="33"/>
+      <c r="M14" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N14" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O14" s="29"/>
       <c r="P14" s="29"/>
@@ -27893,6 +27919,8 @@
     </row>
     <row r="15">
       <c r="C15" s="39"/>
+      <c r="E15" s="29"/>
+      <c r="N15" s="29"/>
     </row>
     <row r="16">
       <c r="A16" s="54" t="s">
@@ -27910,42 +27938,21 @@
       <c r="E16" s="29" t="s">
         <v>631</v>
       </c>
-      <c r="F16" s="9"/>
       <c r="G16" s="29" t="s">
         <v>632</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
       <c r="J16" s="8" t="s">
         <v>678</v>
       </c>
-      <c r="K16" s="9"/>
       <c r="L16" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M16" s="9"/>
+      <c r="M16" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N16" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="9"/>
-      <c r="V16" s="9"/>
-      <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="9"/>
-      <c r="Z16" s="9"/>
-      <c r="AA16" s="9"/>
-      <c r="AB16" s="9"/>
-      <c r="AC16" s="9"/>
-      <c r="AD16" s="9"/>
-      <c r="AE16" s="9"/>
-      <c r="AF16" s="9"/>
-      <c r="AG16" s="9"/>
+        <v>87</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="54" t="s">
@@ -27963,40 +27970,19 @@
       <c r="E17" s="29" t="s">
         <v>631</v>
       </c>
-      <c r="F17" s="9"/>
       <c r="G17" s="29" t="s">
         <v>632</v>
       </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
       <c r="L17" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M17" s="9"/>
+      <c r="M17" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N17" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O17" s="41"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9"/>
-      <c r="Z17" s="9"/>
-      <c r="AA17" s="9"/>
-      <c r="AB17" s="9"/>
-      <c r="AC17" s="9"/>
-      <c r="AD17" s="9"/>
-      <c r="AE17" s="9"/>
-      <c r="AF17" s="9"/>
-      <c r="AG17" s="9"/>
     </row>
     <row r="18">
       <c r="A18" s="54" t="s">
@@ -28014,40 +28000,19 @@
       <c r="E18" s="29" t="s">
         <v>631</v>
       </c>
-      <c r="F18" s="9"/>
       <c r="G18" s="29" t="s">
         <v>632</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
       <c r="L18" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M18" s="9"/>
+      <c r="M18" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N18" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O18" s="41"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
-      <c r="X18" s="9"/>
-      <c r="Y18" s="9"/>
-      <c r="Z18" s="9"/>
-      <c r="AA18" s="9"/>
-      <c r="AB18" s="9"/>
-      <c r="AC18" s="9"/>
-      <c r="AD18" s="9"/>
-      <c r="AE18" s="9"/>
-      <c r="AF18" s="9"/>
-      <c r="AG18" s="9"/>
     </row>
     <row r="19">
       <c r="A19" s="54" t="s">
@@ -28065,40 +28030,19 @@
       <c r="E19" s="29" t="s">
         <v>631</v>
       </c>
-      <c r="F19" s="9"/>
       <c r="G19" s="29" t="s">
         <v>632</v>
       </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
       <c r="L19" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M19" s="9"/>
+      <c r="M19" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N19" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O19" s="41"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="9"/>
-      <c r="AA19" s="9"/>
-      <c r="AB19" s="9"/>
-      <c r="AC19" s="9"/>
-      <c r="AD19" s="9"/>
-      <c r="AE19" s="9"/>
-      <c r="AF19" s="9"/>
-      <c r="AG19" s="9"/>
     </row>
     <row r="20">
       <c r="A20" s="54" t="s">
@@ -28116,40 +28060,19 @@
       <c r="E20" s="29" t="s">
         <v>631</v>
       </c>
-      <c r="F20" s="9"/>
       <c r="G20" s="29" t="s">
         <v>632</v>
       </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
       <c r="L20" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M20" s="9"/>
+      <c r="M20" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N20" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O20" s="41"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="9"/>
-      <c r="AA20" s="9"/>
-      <c r="AB20" s="9"/>
-      <c r="AC20" s="9"/>
-      <c r="AD20" s="9"/>
-      <c r="AE20" s="9"/>
-      <c r="AF20" s="9"/>
-      <c r="AG20" s="9"/>
     </row>
     <row r="21">
       <c r="A21" s="54" t="s">
@@ -28167,40 +28090,19 @@
       <c r="E21" s="29" t="s">
         <v>631</v>
       </c>
-      <c r="F21" s="9"/>
       <c r="G21" s="29" t="s">
         <v>632</v>
       </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
       <c r="L21" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M21" s="9"/>
+      <c r="M21" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N21" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O21" s="41"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
-      <c r="AA21" s="9"/>
-      <c r="AB21" s="9"/>
-      <c r="AC21" s="9"/>
-      <c r="AD21" s="9"/>
-      <c r="AE21" s="9"/>
-      <c r="AF21" s="9"/>
-      <c r="AG21" s="9"/>
     </row>
     <row r="22">
       <c r="A22" s="54" t="s">
@@ -28218,40 +28120,19 @@
       <c r="E22" s="29" t="s">
         <v>631</v>
       </c>
-      <c r="F22" s="9"/>
       <c r="G22" s="29" t="s">
         <v>632</v>
       </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
       <c r="L22" s="33">
         <v>45586.0</v>
       </c>
-      <c r="M22" s="9"/>
+      <c r="M22" s="33">
+        <v>45886.0</v>
+      </c>
       <c r="N22" s="29" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="O22" s="41"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="9"/>
-      <c r="Z22" s="9"/>
-      <c r="AA22" s="9"/>
-      <c r="AB22" s="9"/>
-      <c r="AC22" s="9"/>
-      <c r="AD22" s="9"/>
-      <c r="AE22" s="9"/>
-      <c r="AF22" s="9"/>
-      <c r="AG22" s="9"/>
     </row>
     <row r="23">
       <c r="B23" s="40"/>

</xml_diff>

<commit_message>
Adds EU-GDPR Purpose Compatibility, Proportionality
- Adds concepts for Purpose Compatibility to EU-GDPR (as a module)
- closes #298
- Adds concepts for Proportionality to EU-GDPR (as a module)
- closes #386

Co-authored-by: Stratis Koulierakis <StrKoulierakis@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/eu-gdpr.xlsx
+++ b/code/vocab_csv/eu-gdpr.xlsx
@@ -3,24 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="GDPR_Mapping" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="GDPR_MiscConcepts" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="GDPR_LegalBasis" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="GDPR_LegalBasis_SpecialCategory" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="GDPR_LegalBasis_DataTransfer" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="GDPR_LegalRights" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="GDPR_LegalRights_Justifications" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="GDPR_LegalRights_Impacts" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="GDPR_LegalBasis_Rights_Mapping" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="GDPR_DataTransfers" sheetId="10" r:id="rId13"/>
-    <sheet state="visible" name="GDPR_DPIA" sheetId="11" r:id="rId14"/>
-    <sheet state="visible" name="GDPR_DPIA_properties" sheetId="12" r:id="rId15"/>
-    <sheet state="visible" name="GDPR_DataBreach" sheetId="13" r:id="rId16"/>
-    <sheet state="visible" name="GDPR_compliance" sheetId="14" r:id="rId17"/>
-    <sheet state="visible" name="GDPR_principles" sheetId="15" r:id="rId18"/>
-    <sheet state="visible" name="GDPR_entities" sheetId="16" r:id="rId19"/>
-    <sheet state="visible" name="GDPR_entities_properties" sheetId="17" r:id="rId20"/>
-    <sheet state="visible" name="GDPR_purpose_compatibility" sheetId="18" r:id="rId21"/>
+    <sheet state="visible" name="GDPR_Mapping" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="GDPR_MiscConcepts" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="GDPR_LegalBasis" sheetId="3" r:id="rId7"/>
+    <sheet state="visible" name="GDPR_LegalBasis_SpecialCategory" sheetId="4" r:id="rId8"/>
+    <sheet state="visible" name="GDPR_LegalBasis_DataTransfer" sheetId="5" r:id="rId9"/>
+    <sheet state="visible" name="GDPR_LegalRights" sheetId="6" r:id="rId10"/>
+    <sheet state="visible" name="GDPR_LegalRights_Justifications" sheetId="7" r:id="rId11"/>
+    <sheet state="visible" name="GDPR_LegalRights_Impacts" sheetId="8" r:id="rId12"/>
+    <sheet state="visible" name="GDPR_LegalBasis_Rights_Mapping" sheetId="9" r:id="rId13"/>
+    <sheet state="visible" name="GDPR_DataTransfers" sheetId="10" r:id="rId14"/>
+    <sheet state="visible" name="GDPR_DPIA" sheetId="11" r:id="rId15"/>
+    <sheet state="visible" name="GDPR_DPIA_properties" sheetId="12" r:id="rId16"/>
+    <sheet state="visible" name="GDPR_DataBreach" sheetId="13" r:id="rId17"/>
+    <sheet state="visible" name="GDPR_compliance" sheetId="14" r:id="rId18"/>
+    <sheet state="visible" name="GDPR_principles" sheetId="15" r:id="rId19"/>
+    <sheet state="visible" name="GDPR_entities" sheetId="16" r:id="rId20"/>
+    <sheet state="visible" name="GDPR_entities_properties" sheetId="17" r:id="rId21"/>
+    <sheet state="visible" name="GDPR_purpose_compatibility" sheetId="18" r:id="rId22"/>
+    <sheet state="visible" name="GDPR_proportionality" sheetId="19" r:id="rId23"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2591" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2664" uniqueCount="1169">
   <si>
     <t>Concept</t>
   </si>
@@ -372,7 +373,7 @@
     <t>Cross Border Processing</t>
   </si>
   <si>
-    <t>‘Cross-Border Processing’ means either: (a) processing of personal data which takes place in the context of the activities of establishments in more than one Member State of a controller or processor in the Union where the controller or processor is established in more than one Member State; or (b)  processing of personal data which takes place in the context of the activities of a single establishment of a controller or processor in the Union but which substantially affects or is likely to substantially affect data subjects in more than one Member State</t>
+    <t>‘Cross-Border Processing’ means either: (a) processing of personal data which takes place in the context of the activities of establishments in more than one Member State of a controller or processor in the Union where the controller or processor is established in more than one Member State; or (b) processing of personal data which takes place in the context of the activities of a single establishment of a controller or processor in the Union but which substantially affects or is likely to substantially affect data subjects in more than one Member State</t>
   </si>
   <si>
     <t>InformationSocietyService</t>
@@ -3614,13 +3615,13 @@
     <t>Purpose Compatibility</t>
   </si>
   <si>
-    <t>An assessment of the compatbility with a specific Purpose of processing personal data as defined and interpreted under the GDPR</t>
+    <t>Status representing the compatibility of the new purpose with the principle of purpose limitation according to the GDPR</t>
   </si>
   <si>
     <t>dpv:ReuseCompatibility</t>
   </si>
   <si>
-    <t>Harshvardhan J. Pandit, Georg P. Krog, Julian Flake, Delaram Golpayegani, Beatriz Esteves, Paul Ryan, Arthit Suriyawongkul, Julio Hernandez</t>
+    <t>Harshvardhan J. Pandit, Georg P. Krog, Julian Flake, Delaram Golpayegani, Beatriz Esteves, Paul Ryan, Arthit Suriyawongkul, Julio Hernandez, Stratis Koulierakis</t>
   </si>
   <si>
     <t>PurposeCompatible</t>
@@ -3629,13 +3630,13 @@
     <t>Purpose Compatible</t>
   </si>
   <si>
-    <t>An assessment that the specified use or purpose is compatible with the Purpose of processing personal data as defined and interpreted under the GDPR</t>
-  </si>
-  <si>
-    <t>dpv:PrimaryUse</t>
-  </si>
-  <si>
-    <t>eu-gdpr:PurposeCompatibility</t>
+    <t>Status representing the new purpose is compatible with the principle of purpose limitation according to the GDPR</t>
+  </si>
+  <si>
+    <t>dpv:PrimaryUse,eu-gdpr:PurposeCompatibility</t>
+  </si>
+  <si>
+    <t>A compatible purpose can allow for continued use of the same legal basis without any changes</t>
   </si>
   <si>
     <t>PurposeIncompatible</t>
@@ -3644,10 +3645,117 @@
     <t>Purpose Incompatible</t>
   </si>
   <si>
-    <t>An assessment that the specified use or purpose is incompatible with the Purpose of processing personal data as defined and interpreted under the GDPR</t>
-  </si>
-  <si>
-    <t>dpv:SecondaryUse</t>
+    <t>Status representing the new purpose is incompatible with the principle of purpose limitation according to the GDPR</t>
+  </si>
+  <si>
+    <t>dpv:SecondaryUse,eu-gdpr:PurposeCompatibility</t>
+  </si>
+  <si>
+    <t>An incompatible purpose means the process cannot be continued without a new valid legal basis</t>
+  </si>
+  <si>
+    <t>PurposeCompatibilityAssessment</t>
+  </si>
+  <si>
+    <t>Purpose Compatibility Assessment</t>
+  </si>
+  <si>
+    <t>An assessment for evaluating the compatibility of the new purpose with the principle of purpose limitation according to the GDPR</t>
+  </si>
+  <si>
+    <t>dpv:Assessment</t>
+  </si>
+  <si>
+    <t>ProportionalityAssessment</t>
+  </si>
+  <si>
+    <t>Proportionality Assessment</t>
+  </si>
+  <si>
+    <t>Proportionality is a general principle of EU law, which when applied for the GDPR requires striking a balance between the processing of personal data and the resulting impacts on rights. More simply, the processing should not result in a disproportionate impact on rights</t>
+  </si>
+  <si>
+    <t>dpv:ImpactAssessment</t>
+  </si>
+  <si>
+    <t>The assessment of proportionality requires an assessment of suitability (represented by `eu-gdpr:SuitabilityAssessment`), necessity (represented by `eu-gdpr:NecessityAssessment`), and a balancing test (represented by `eu-gdpr:BalancingTest`). The outcome of the proportionality assessment is represented as an instance of `eu-gdpr:ProportionalityStatus`</t>
+  </si>
+  <si>
+    <t>Stratis Koulierakis, Georg P. Krog, Harshvardhan J. Pandit</t>
+  </si>
+  <si>
+    <t>SuitabilityAssessment</t>
+  </si>
+  <si>
+    <t>Suitability Assessment</t>
+  </si>
+  <si>
+    <t>An assessment of whether the processing of personal data is suitable to achieve the stated aims</t>
+  </si>
+  <si>
+    <t>dpv:Assessment,eu-gdpr:ProportionalityAssessment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While Suitability Assessment can be carried out on its own, it is an integral part of the Proportionality Assessment process
+</t>
+  </si>
+  <si>
+    <t>Stratis Koulierakis</t>
+  </si>
+  <si>
+    <t>NecessityAssessment</t>
+  </si>
+  <si>
+    <t>Necessity Assessment</t>
+  </si>
+  <si>
+    <t>An assessment of whether the processing of personal data is necessary to achieve the stated aims, where necessary indicates a lack of other means which could have been used instead</t>
+  </si>
+  <si>
+    <t>While Necessity can be assessed on its own, it is an integral part of the Proportionality Assessment process</t>
+  </si>
+  <si>
+    <t>BalancingTest</t>
+  </si>
+  <si>
+    <t>Balancing Test</t>
+  </si>
+  <si>
+    <t>An assessment of whether the individual's interests override the interests of the controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While Balancing Test can be conducted on its own, it is an integral part of the Proportionality Assessment process
+</t>
+  </si>
+  <si>
+    <t>ProportionalityStatus</t>
+  </si>
+  <si>
+    <t>Proportionality Status</t>
+  </si>
+  <si>
+    <t>Status indicating whether the specific activity or context is proportionate</t>
+  </si>
+  <si>
+    <t>dpv:Status</t>
+  </si>
+  <si>
+    <t>Proportionate</t>
+  </si>
+  <si>
+    <t>Status representing the activity or context is proportionate</t>
+  </si>
+  <si>
+    <t>eu-gdpr:ProportionalityStatus</t>
+  </si>
+  <si>
+    <t>Disproportionate</t>
+  </si>
+  <si>
+    <t>Status representing the activity or context is disproportionate i.e. it is not proportionate</t>
+  </si>
+  <si>
+    <t>A Disproportinate status indicates that the process should not be continued as it risks impacting the rights of the data subject in an unacceptable manner</t>
   </si>
 </sst>
 </file>
@@ -3891,7 +3999,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="111">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -4173,23 +4281,47 @@
     <xf borderId="0" fillId="2" fontId="29" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4288,6 +4420,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
@@ -4318,6 +4454,10 @@
 
 <file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17587,6 +17727,674 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="2" width="17.25"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="93" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="94" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="95" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="95" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="95" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="95" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="95" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="96" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="97" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="98"/>
+      <c r="Y1" s="98"/>
+      <c r="Z1" s="98"/>
+      <c r="AA1" s="98"/>
+      <c r="AB1" s="98"/>
+      <c r="AC1" s="98"/>
+      <c r="AD1" s="98"/>
+      <c r="AE1" s="98"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="99" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B2" s="100" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C2" s="100" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D2" s="101"/>
+      <c r="E2" s="100" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="102">
+        <v>45940.0</v>
+      </c>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100" t="s">
+        <v>1124</v>
+      </c>
+      <c r="M2" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101"/>
+      <c r="S2" s="101"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="101"/>
+      <c r="V2" s="101"/>
+      <c r="W2" s="101"/>
+      <c r="X2" s="101"/>
+      <c r="Y2" s="101"/>
+      <c r="Z2" s="101"/>
+      <c r="AA2" s="101"/>
+      <c r="AB2" s="101"/>
+      <c r="AC2" s="101"/>
+      <c r="AD2" s="101"/>
+      <c r="AE2" s="101"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="104" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B3" s="104" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C3" s="104" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D3" s="100" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E3" s="100" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G3" s="101"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="100" t="s">
+        <v>1129</v>
+      </c>
+      <c r="J3" s="102">
+        <v>45940.0</v>
+      </c>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100" t="s">
+        <v>1124</v>
+      </c>
+      <c r="M3" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="101"/>
+      <c r="O3" s="101"/>
+      <c r="P3" s="101"/>
+      <c r="Q3" s="101"/>
+      <c r="R3" s="101"/>
+      <c r="S3" s="101"/>
+      <c r="T3" s="101"/>
+      <c r="U3" s="101"/>
+      <c r="V3" s="101"/>
+      <c r="W3" s="101"/>
+      <c r="X3" s="101"/>
+      <c r="Y3" s="101"/>
+      <c r="Z3" s="101"/>
+      <c r="AA3" s="101"/>
+      <c r="AB3" s="101"/>
+      <c r="AC3" s="101"/>
+      <c r="AD3" s="101"/>
+      <c r="AE3" s="101"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="104" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B4" s="106" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C4" s="104" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D4" s="100" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E4" s="100" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G4" s="101"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="100" t="s">
+        <v>1134</v>
+      </c>
+      <c r="J4" s="102">
+        <v>45940.0</v>
+      </c>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100" t="s">
+        <v>1124</v>
+      </c>
+      <c r="M4" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="101"/>
+      <c r="O4" s="101"/>
+      <c r="P4" s="101"/>
+      <c r="Q4" s="101"/>
+      <c r="R4" s="101"/>
+      <c r="S4" s="101"/>
+      <c r="T4" s="101"/>
+      <c r="U4" s="101"/>
+      <c r="V4" s="101"/>
+      <c r="W4" s="101"/>
+      <c r="X4" s="101"/>
+      <c r="Y4" s="101"/>
+      <c r="Z4" s="101"/>
+      <c r="AA4" s="101"/>
+      <c r="AB4" s="101"/>
+      <c r="AC4" s="101"/>
+      <c r="AD4" s="101"/>
+      <c r="AE4" s="101"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="103" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B5" s="103" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C5" s="103" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D5" s="103" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E5" s="103" t="s">
+        <v>428</v>
+      </c>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="102">
+        <v>45940.0</v>
+      </c>
+      <c r="K5" s="103"/>
+      <c r="L5" s="103" t="s">
+        <v>1124</v>
+      </c>
+      <c r="M5" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="107"/>
+      <c r="O5" s="107"/>
+      <c r="P5" s="107"/>
+      <c r="Q5" s="107"/>
+      <c r="R5" s="107"/>
+      <c r="S5" s="107"/>
+      <c r="T5" s="107"/>
+      <c r="U5" s="107"/>
+      <c r="V5" s="107"/>
+      <c r="W5" s="107"/>
+      <c r="X5" s="107"/>
+      <c r="Y5" s="107"/>
+      <c r="Z5" s="107"/>
+      <c r="AA5" s="107"/>
+      <c r="AB5" s="107"/>
+      <c r="AC5" s="107"/>
+      <c r="AD5" s="107"/>
+      <c r="AE5" s="107"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="107"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="107"/>
+      <c r="M6" s="107"/>
+      <c r="N6" s="107"/>
+      <c r="O6" s="107"/>
+      <c r="P6" s="107"/>
+      <c r="Q6" s="107"/>
+      <c r="R6" s="107"/>
+      <c r="S6" s="107"/>
+      <c r="T6" s="107"/>
+      <c r="U6" s="107"/>
+      <c r="V6" s="107"/>
+      <c r="W6" s="107"/>
+      <c r="X6" s="107"/>
+      <c r="Y6" s="107"/>
+      <c r="Z6" s="107"/>
+      <c r="AA6" s="107"/>
+      <c r="AB6" s="107"/>
+      <c r="AC6" s="107"/>
+      <c r="AD6" s="107"/>
+      <c r="AE6" s="107"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="107"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="107"/>
+      <c r="N7" s="107"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="107"/>
+      <c r="Q7" s="107"/>
+      <c r="R7" s="107"/>
+      <c r="S7" s="107"/>
+      <c r="T7" s="107"/>
+      <c r="U7" s="107"/>
+      <c r="V7" s="107"/>
+      <c r="W7" s="107"/>
+      <c r="X7" s="107"/>
+      <c r="Y7" s="107"/>
+      <c r="Z7" s="107"/>
+      <c r="AA7" s="107"/>
+      <c r="AB7" s="107"/>
+      <c r="AC7" s="107"/>
+      <c r="AD7" s="107"/>
+      <c r="AE7" s="107"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="107"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="107"/>
+      <c r="H8" s="107"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
+      <c r="K8" s="107"/>
+      <c r="L8" s="107"/>
+      <c r="M8" s="107"/>
+      <c r="N8" s="107"/>
+      <c r="O8" s="107"/>
+      <c r="P8" s="107"/>
+      <c r="Q8" s="107"/>
+      <c r="R8" s="107"/>
+      <c r="S8" s="107"/>
+      <c r="T8" s="107"/>
+      <c r="U8" s="107"/>
+      <c r="V8" s="107"/>
+      <c r="W8" s="107"/>
+      <c r="X8" s="107"/>
+      <c r="Y8" s="107"/>
+      <c r="Z8" s="107"/>
+      <c r="AA8" s="107"/>
+      <c r="AB8" s="107"/>
+      <c r="AC8" s="107"/>
+      <c r="AD8" s="107"/>
+      <c r="AE8" s="107"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="107"/>
+      <c r="B9" s="107"/>
+      <c r="C9" s="107"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="100"/>
+      <c r="G9" s="107"/>
+      <c r="H9" s="107"/>
+      <c r="I9" s="107"/>
+      <c r="J9" s="107"/>
+      <c r="K9" s="107"/>
+      <c r="L9" s="107"/>
+      <c r="M9" s="107"/>
+      <c r="N9" s="107"/>
+      <c r="O9" s="107"/>
+      <c r="P9" s="107"/>
+      <c r="Q9" s="107"/>
+      <c r="R9" s="107"/>
+      <c r="S9" s="107"/>
+      <c r="T9" s="107"/>
+      <c r="U9" s="107"/>
+      <c r="V9" s="107"/>
+      <c r="W9" s="107"/>
+      <c r="X9" s="107"/>
+      <c r="Y9" s="107"/>
+      <c r="Z9" s="107"/>
+      <c r="AA9" s="107"/>
+      <c r="AB9" s="107"/>
+      <c r="AC9" s="107"/>
+      <c r="AD9" s="107"/>
+      <c r="AE9" s="107"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="107"/>
+      <c r="B10" s="107"/>
+      <c r="C10" s="107"/>
+      <c r="D10" s="107"/>
+      <c r="E10" s="107"/>
+      <c r="F10" s="107"/>
+      <c r="G10" s="107"/>
+      <c r="H10" s="107"/>
+      <c r="I10" s="107"/>
+      <c r="J10" s="107"/>
+      <c r="K10" s="107"/>
+      <c r="L10" s="107"/>
+      <c r="M10" s="107"/>
+      <c r="N10" s="107"/>
+      <c r="O10" s="107"/>
+      <c r="P10" s="107"/>
+      <c r="Q10" s="107"/>
+      <c r="R10" s="107"/>
+      <c r="S10" s="107"/>
+      <c r="T10" s="107"/>
+      <c r="U10" s="107"/>
+      <c r="V10" s="107"/>
+      <c r="W10" s="107"/>
+      <c r="X10" s="107"/>
+      <c r="Y10" s="107"/>
+      <c r="Z10" s="107"/>
+      <c r="AA10" s="107"/>
+      <c r="AB10" s="107"/>
+      <c r="AC10" s="107"/>
+      <c r="AD10" s="107"/>
+      <c r="AE10" s="107"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="107"/>
+      <c r="B11" s="107"/>
+      <c r="C11" s="107"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="107"/>
+      <c r="G11" s="107"/>
+      <c r="H11" s="107"/>
+      <c r="I11" s="107"/>
+      <c r="J11" s="107"/>
+      <c r="K11" s="107"/>
+      <c r="L11" s="107"/>
+      <c r="M11" s="107"/>
+      <c r="N11" s="107"/>
+      <c r="O11" s="107"/>
+      <c r="P11" s="107"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="107"/>
+      <c r="S11" s="107"/>
+      <c r="T11" s="107"/>
+      <c r="U11" s="107"/>
+      <c r="V11" s="107"/>
+      <c r="W11" s="107"/>
+      <c r="X11" s="107"/>
+      <c r="Y11" s="107"/>
+      <c r="Z11" s="107"/>
+      <c r="AA11" s="107"/>
+      <c r="AB11" s="107"/>
+      <c r="AC11" s="107"/>
+      <c r="AD11" s="107"/>
+      <c r="AE11" s="107"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="107"/>
+      <c r="B12" s="107"/>
+      <c r="C12" s="107"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="107"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="107"/>
+      <c r="K12" s="107"/>
+      <c r="L12" s="107"/>
+      <c r="M12" s="107"/>
+      <c r="N12" s="107"/>
+      <c r="O12" s="107"/>
+      <c r="P12" s="107"/>
+      <c r="Q12" s="107"/>
+      <c r="R12" s="107"/>
+      <c r="S12" s="107"/>
+      <c r="T12" s="107"/>
+      <c r="U12" s="107"/>
+      <c r="V12" s="107"/>
+      <c r="W12" s="107"/>
+      <c r="X12" s="107"/>
+      <c r="Y12" s="107"/>
+      <c r="Z12" s="107"/>
+      <c r="AA12" s="107"/>
+      <c r="AB12" s="107"/>
+      <c r="AC12" s="107"/>
+      <c r="AD12" s="107"/>
+      <c r="AE12" s="107"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="107"/>
+      <c r="B13" s="107"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="107"/>
+      <c r="F13" s="107"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="107"/>
+      <c r="I13" s="107"/>
+      <c r="J13" s="107"/>
+      <c r="K13" s="107"/>
+      <c r="L13" s="107"/>
+      <c r="M13" s="107"/>
+      <c r="N13" s="107"/>
+      <c r="O13" s="107"/>
+      <c r="P13" s="107"/>
+      <c r="Q13" s="107"/>
+      <c r="R13" s="107"/>
+      <c r="S13" s="107"/>
+      <c r="T13" s="107"/>
+      <c r="U13" s="107"/>
+      <c r="V13" s="107"/>
+      <c r="W13" s="107"/>
+      <c r="X13" s="107"/>
+      <c r="Y13" s="107"/>
+      <c r="Z13" s="107"/>
+      <c r="AA13" s="107"/>
+      <c r="AB13" s="107"/>
+      <c r="AC13" s="107"/>
+      <c r="AD13" s="107"/>
+      <c r="AE13" s="107"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="107"/>
+      <c r="B14" s="107"/>
+      <c r="C14" s="107"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="107"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="107"/>
+      <c r="H14" s="107"/>
+      <c r="I14" s="107"/>
+      <c r="J14" s="107"/>
+      <c r="K14" s="107"/>
+      <c r="L14" s="107"/>
+      <c r="M14" s="107"/>
+      <c r="N14" s="107"/>
+      <c r="O14" s="107"/>
+      <c r="P14" s="107"/>
+      <c r="Q14" s="107"/>
+      <c r="R14" s="107"/>
+      <c r="S14" s="107"/>
+      <c r="T14" s="107"/>
+      <c r="U14" s="107"/>
+      <c r="V14" s="107"/>
+      <c r="W14" s="107"/>
+      <c r="X14" s="107"/>
+      <c r="Y14" s="107"/>
+      <c r="Z14" s="107"/>
+      <c r="AA14" s="107"/>
+      <c r="AB14" s="107"/>
+      <c r="AC14" s="107"/>
+      <c r="AD14" s="107"/>
+      <c r="AE14" s="107"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="107"/>
+      <c r="B15" s="107"/>
+      <c r="C15" s="107"/>
+      <c r="D15" s="107"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="107"/>
+      <c r="G15" s="107"/>
+      <c r="H15" s="107"/>
+      <c r="I15" s="107"/>
+      <c r="J15" s="107"/>
+      <c r="K15" s="107"/>
+      <c r="L15" s="107"/>
+      <c r="M15" s="107"/>
+      <c r="N15" s="107"/>
+      <c r="O15" s="107"/>
+      <c r="P15" s="107"/>
+      <c r="Q15" s="107"/>
+      <c r="R15" s="107"/>
+      <c r="S15" s="107"/>
+      <c r="T15" s="107"/>
+      <c r="U15" s="107"/>
+      <c r="V15" s="107"/>
+      <c r="W15" s="107"/>
+      <c r="X15" s="107"/>
+      <c r="Y15" s="107"/>
+      <c r="Z15" s="107"/>
+      <c r="AA15" s="107"/>
+      <c r="AB15" s="107"/>
+      <c r="AC15" s="107"/>
+      <c r="AD15" s="107"/>
+      <c r="AE15" s="107"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="107"/>
+      <c r="B16" s="107"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="107"/>
+      <c r="F16" s="107"/>
+      <c r="G16" s="107"/>
+      <c r="H16" s="107"/>
+      <c r="I16" s="107"/>
+      <c r="J16" s="107"/>
+      <c r="K16" s="107"/>
+      <c r="L16" s="107"/>
+      <c r="M16" s="107"/>
+      <c r="N16" s="107"/>
+      <c r="O16" s="107"/>
+      <c r="P16" s="107"/>
+      <c r="Q16" s="107"/>
+      <c r="R16" s="107"/>
+      <c r="S16" s="107"/>
+      <c r="T16" s="107"/>
+      <c r="U16" s="107"/>
+      <c r="V16" s="107"/>
+      <c r="W16" s="107"/>
+      <c r="X16" s="107"/>
+      <c r="Y16" s="107"/>
+      <c r="Z16" s="107"/>
+      <c r="AA16" s="107"/>
+      <c r="AB16" s="107"/>
+      <c r="AC16" s="107"/>
+      <c r="AD16" s="107"/>
+      <c r="AE16" s="107"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="107"/>
+      <c r="B17" s="107"/>
+      <c r="C17" s="107"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="107"/>
+      <c r="J17" s="107"/>
+      <c r="K17" s="107"/>
+      <c r="L17" s="107"/>
+      <c r="M17" s="107"/>
+      <c r="N17" s="107"/>
+      <c r="O17" s="107"/>
+      <c r="P17" s="107"/>
+      <c r="Q17" s="107"/>
+      <c r="R17" s="107"/>
+      <c r="S17" s="107"/>
+      <c r="T17" s="107"/>
+      <c r="U17" s="107"/>
+      <c r="V17" s="107"/>
+      <c r="W17" s="107"/>
+      <c r="X17" s="107"/>
+      <c r="Y17" s="107"/>
+      <c r="Z17" s="107"/>
+      <c r="AA17" s="107"/>
+      <c r="AB17" s="107"/>
+      <c r="AC17" s="107"/>
+      <c r="AD17" s="107"/>
+      <c r="AE17" s="107"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
     <col customWidth="1" min="2" max="2" width="17.25"/>
   </cols>
   <sheetData>
@@ -17627,51 +18435,55 @@
       <c r="L1" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="97"/>
-      <c r="S1" s="97"/>
-      <c r="T1" s="97"/>
-      <c r="U1" s="97"/>
-      <c r="V1" s="97"/>
-      <c r="W1" s="97"/>
-      <c r="X1" s="97"/>
-      <c r="Y1" s="97"/>
-      <c r="Z1" s="97"/>
-      <c r="AA1" s="97"/>
-      <c r="AB1" s="97"/>
-      <c r="AC1" s="97"/>
-      <c r="AD1" s="97"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="98"/>
+      <c r="Y1" s="98"/>
+      <c r="Z1" s="98"/>
+      <c r="AA1" s="98"/>
+      <c r="AB1" s="98"/>
+      <c r="AC1" s="98"/>
+      <c r="AD1" s="98"/>
     </row>
     <row r="2">
-      <c r="A2" s="85" t="s">
-        <v>1120</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>1121</v>
+      <c r="A2" s="8" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>1140</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>1122</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>1123</v>
-      </c>
-      <c r="E2" s="51"/>
+        <v>1141</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>428</v>
+      </c>
       <c r="F2" s="51"/>
       <c r="G2" s="51"/>
       <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="98">
-        <v>45827.0</v>
-      </c>
-      <c r="K2" s="51" t="s">
-        <v>1124</v>
-      </c>
-      <c r="L2" s="51" t="s">
-        <v>204</v>
+      <c r="I2" s="50" t="s">
+        <v>1143</v>
+      </c>
+      <c r="J2" s="108">
+        <v>45940.0</v>
+      </c>
+      <c r="K2" s="50" t="s">
+        <v>1144</v>
+      </c>
+      <c r="L2" s="50" t="s">
+        <v>11</v>
       </c>
       <c r="M2" s="51"/>
       <c r="N2" s="51"/>
@@ -17693,33 +18505,35 @@
       <c r="AD2" s="51"/>
     </row>
     <row r="3">
-      <c r="A3" s="99" t="s">
-        <v>1125</v>
-      </c>
-      <c r="B3" s="99" t="s">
-        <v>1126</v>
-      </c>
-      <c r="C3" s="100" t="s">
-        <v>1127</v>
-      </c>
-      <c r="D3" s="51" t="s">
-        <v>1128</v>
+      <c r="A3" s="8" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C3" s="104" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>1148</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>1129</v>
+        <v>428</v>
       </c>
       <c r="F3" s="51"/>
       <c r="G3" s="51"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="98">
-        <v>45827.0</v>
-      </c>
-      <c r="K3" s="51" t="s">
-        <v>1124</v>
-      </c>
-      <c r="L3" s="90" t="s">
-        <v>204</v>
+      <c r="H3" s="109"/>
+      <c r="I3" s="50" t="s">
+        <v>1149</v>
+      </c>
+      <c r="J3" s="108">
+        <v>46059.0</v>
+      </c>
+      <c r="K3" s="50" t="s">
+        <v>1150</v>
+      </c>
+      <c r="L3" s="50" t="s">
+        <v>11</v>
       </c>
       <c r="M3" s="51"/>
       <c r="N3" s="51"/>
@@ -17741,33 +18555,35 @@
       <c r="AD3" s="51"/>
     </row>
     <row r="4">
-      <c r="A4" s="99" t="s">
-        <v>1130</v>
-      </c>
-      <c r="B4" s="102" t="s">
-        <v>1131</v>
-      </c>
-      <c r="C4" s="100" t="s">
-        <v>1132</v>
-      </c>
-      <c r="D4" s="51" t="s">
-        <v>1133</v>
+      <c r="A4" s="8" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C4" s="104" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>1148</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>1129</v>
+        <v>428</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="51"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="98">
-        <v>45827.0</v>
-      </c>
-      <c r="K4" s="51" t="s">
-        <v>1124</v>
-      </c>
-      <c r="L4" s="90" t="s">
-        <v>204</v>
+      <c r="H4" s="109"/>
+      <c r="I4" s="50" t="s">
+        <v>1154</v>
+      </c>
+      <c r="J4" s="108">
+        <v>45940.0</v>
+      </c>
+      <c r="K4" s="50" t="s">
+        <v>1144</v>
+      </c>
+      <c r="L4" s="50" t="s">
+        <v>11</v>
       </c>
       <c r="M4" s="51"/>
       <c r="N4" s="51"/>
@@ -17787,6 +18603,151 @@
       <c r="AB4" s="51"/>
       <c r="AC4" s="51"/>
       <c r="AD4" s="51"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C5" s="110" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>428</v>
+      </c>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="50" t="s">
+        <v>1158</v>
+      </c>
+      <c r="J5" s="108">
+        <v>45940.0</v>
+      </c>
+      <c r="K5" s="50" t="s">
+        <v>1144</v>
+      </c>
+      <c r="L5" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="51"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="51"/>
+      <c r="U5" s="51"/>
+      <c r="V5" s="51"/>
+      <c r="W5" s="51"/>
+      <c r="X5" s="51"/>
+      <c r="Y5" s="51"/>
+      <c r="Z5" s="51"/>
+      <c r="AA5" s="51"/>
+      <c r="AB5" s="51"/>
+      <c r="AC5" s="51"/>
+      <c r="AD5" s="51"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C6" s="110" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D6" s="51"/>
+      <c r="E6" s="50" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="108">
+        <v>45940.0</v>
+      </c>
+      <c r="K6" s="50" t="s">
+        <v>1144</v>
+      </c>
+      <c r="L6" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="51"/>
+      <c r="R6" s="51"/>
+      <c r="S6" s="51"/>
+      <c r="T6" s="51"/>
+      <c r="U6" s="51"/>
+      <c r="V6" s="51"/>
+      <c r="W6" s="51"/>
+      <c r="X6" s="51"/>
+      <c r="Y6" s="51"/>
+      <c r="Z6" s="51"/>
+      <c r="AA6" s="51"/>
+      <c r="AB6" s="51"/>
+      <c r="AC6" s="51"/>
+      <c r="AD6" s="51"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>1165</v>
+      </c>
+      <c r="J7" s="108">
+        <v>45940.0</v>
+      </c>
+      <c r="K7" s="50" t="s">
+        <v>1144</v>
+      </c>
+      <c r="L7" s="50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>1165</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>1168</v>
+      </c>
+      <c r="J8" s="108">
+        <v>45940.0</v>
+      </c>
+      <c r="K8" s="50" t="s">
+        <v>1144</v>
+      </c>
+      <c r="L8" s="50" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Corrected name for Efstratios in EU-GDPR
Stratis -> Efstratios
</commit_message>
<xml_diff>
--- a/code/vocab_csv/eu-gdpr.xlsx
+++ b/code/vocab_csv/eu-gdpr.xlsx
@@ -3621,7 +3621,7 @@
     <t>dpv:ReuseCompatibility</t>
   </si>
   <si>
-    <t>Harshvardhan J. Pandit, Georg P. Krog, Julian Flake, Delaram Golpayegani, Beatriz Esteves, Paul Ryan, Arthit Suriyawongkul, Julio Hernandez, Stratis Koulierakis</t>
+    <t>Harshvardhan J. Pandit, Georg P. Krog, Julian Flake, Delaram Golpayegani, Beatriz Esteves, Paul Ryan, Arthit Suriyawongkul, Julio Hernandez, Efstratios Koulierakis</t>
   </si>
   <si>
     <t>PurposeCompatible</t>
@@ -3681,7 +3681,7 @@
     <t>The assessment of proportionality requires an assessment of suitability (represented by `eu-gdpr:SuitabilityAssessment`), necessity (represented by `eu-gdpr:NecessityAssessment`), and a balancing test (represented by `eu-gdpr:BalancingTest`). The outcome of the proportionality assessment is represented as an instance of `eu-gdpr:ProportionalityStatus`</t>
   </si>
   <si>
-    <t>Stratis Koulierakis, Georg P. Krog, Harshvardhan J. Pandit</t>
+    <t>Efstratios Koulierakis, Georg P. Krog, Harshvardhan J. Pandit</t>
   </si>
   <si>
     <t>SuitabilityAssessment</t>
@@ -3700,7 +3700,7 @@
 </t>
   </si>
   <si>
-    <t>Stratis Koulierakis</t>
+    <t>Efstratios Koulierakis</t>
   </si>
   <si>
     <t>NecessityAssessment</t>

</xml_diff>